<commit_message>
excel test ver 4
</commit_message>
<xml_diff>
--- a/c_wrk/test.xlsx
+++ b/c_wrk/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t xml:space="preserve">host/minilua.c:4348:10: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
 host/minilua.c:4590:9: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
@@ -36,6 +36,130 @@
 lib_string.c:687:7: warning: Dereference of null pointer [core.NullDereference]
 luajit.c:284:34: warning: Null pointer passed to 1st parameter expecting 'nonnull' [core.NonNullParamChecker]
 </t>
+  </si>
+  <si>
+    <t>no value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lj_snap.c:566:8: warning: Value stored to 'tmp' is never read [deadcode.DeadStores]
+lj_crecord.c:247:2: warning: Value stored to 'step' is never read [deadcode.DeadStores]
+./lj_asm_x86.h:1293:11: warning: Although the value stored to 'osrc' is used in the enclosing expression, the value is never actually read from 'osrc' [deadcode.DeadStores]
+lj_cconv.c:212:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:276:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:283:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:289:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:328:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:503:25: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
+src/http_parser.c:2070:3: warning: Value stored to 'uf' is never read [deadcode.DeadStores]
+</t>
+  </si>
+  <si>
+    <t>host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:697:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:732:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:741:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:744:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:746:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:752:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:754:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:755:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:758:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1294:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1351:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4703:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4904:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6101:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6761:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7567:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7575:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7600:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7605:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7610:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7615:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7631:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1388:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1511:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:181:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:650:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:753:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:754:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2151:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2152:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2153:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:285:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:291:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:315:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:361:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:413:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:479:40: warning: Call to function 'memcpy' is insecure as it does not provide security chec</t>
   </si>
 </sst>
 </file>
@@ -370,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -384,6 +508,51 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel test ver 5
</commit_message>
<xml_diff>
--- a/c_wrk/test.xlsx
+++ b/c_wrk/test.xlsx
@@ -494,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A10"/>
+  <dimension ref="C1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -503,53 +503,35 @@
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="3:12">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel test ver 6
</commit_message>
<xml_diff>
--- a/c_wrk/test.xlsx
+++ b/c_wrk/test.xlsx
@@ -14,152 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">host/minilua.c:4348:10: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
-host/minilua.c:4590:9: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
-lj_strscan.c:309:7: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
-lj_opt_mem.c:46:9: warning: Dereference of null pointer [core.NullDereference]
-lj_opt_narrow.c:374:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
-lj_opt_narrow.c:375:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
-./lj_obj.h:842:5: warning: Undefined or garbage value returned to caller [core.uninitialized.UndefReturn]
-lj_record.c:808:7: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
-lj_record.c:878:11: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
-lj_record.c:878:30: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
-lj_record.c:1166:11: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
-lj_record.c:1783:7: warning: 1st function call argument is an uninitialized value [core.CallAndMessage]
-./lj_asm_x86.h:395:11: warning: Branch condition evaluates to a garbage value [core.uninitialized.Branch]
-./lj_asm_x86.h:455:5: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
-lj_carith.c:158:7: warning: Access to field 'info' results in a dereference of a null pointer [core.NullDereference]
-lj_lib.c:80:12: warning: Dereference of null pointer [core.NullDereference]
-lib_string.c:324:43: warning: Dereference of null pointer (loaded from variable 's') [core.NullDereference]
-lib_string.c:687:7: warning: Dereference of null pointer [core.NullDereference]
-luajit.c:284:34: warning: Null pointer passed to 1st parameter expecting 'nonnull' [core.NonNullParamChecker]
-</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>no value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lj_snap.c:566:8: warning: Value stored to 'tmp' is never read [deadcode.DeadStores]
-lj_crecord.c:247:2: warning: Value stored to 'step' is never read [deadcode.DeadStores]
-./lj_asm_x86.h:1293:11: warning: Although the value stored to 'osrc' is used in the enclosing expression, the value is never actually read from 'osrc' [deadcode.DeadStores]
-lj_cconv.c:212:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
-lj_cconv.c:276:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
-lj_cconv.c:283:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
-lj_cconv.c:289:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
-lj_cconv.c:328:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
-lj_cconv.c:503:25: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
-src/http_parser.c:2070:3: warning: Value stored to 'uf' is never read [deadcode.DeadStores]
-</t>
-  </si>
-  <si>
-    <t>host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:697:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:732:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:741:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-host/minilua.c:744:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
-host/minilua.c:746:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
-host/minilua.c:752:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-host/minilua.c:754:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:755:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
-host/minilua.c:758:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
-host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
-host/minilua.c:1294:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:1351:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:4703:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:4904:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:6101:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:6761:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:7567:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:7575:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-host/minilua.c:7600:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:7605:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:7610:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:7615:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/minilua.c:7631:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
-lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_parse.c:1388:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_parse.c:1511:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_snap.c:181:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_record.c:650:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_record.c:753:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_record.c:754:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_record.c:2151:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_record.c:2152:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_record.c:2153:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_cconv.c:285:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_cconv.c:291:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_cconv.c:315:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_cconv.c:361:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_cconv.c:413:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
-lj_cconv.c:479:40: warning: Call to function 'memcpy' is insecure as it does not provide security chec</t>
   </si>
 </sst>
 </file>
@@ -494,45 +351,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C1:L1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="3" max="12" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:12">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel test ver 7
</commit_message>
<xml_diff>
--- a/c_wrk/test.xlsx
+++ b/c_wrk/test.xlsx
@@ -14,9 +14,417 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+  <si>
+    <t>2018-01-21T06:00:58Z_4.1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host/minilua.c:4349:10: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
+host/minilua.c:4591:9: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_strscan.c:295:5: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_strscan.c:310:7: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_strfmt.c:426:7: warning: 3rd function call argument is an uninitialized value [core.CallAndMessage]
+lj_strfmt_num.c:184:7: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_strfmt_num.c:202:7: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_strfmt_num.c:426:9: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_strfmt_num.c:427:9: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_opt_narrow.c:381:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
+lj_opt_narrow.c:382:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
+./lj_obj.h:965:5: warning: Undefined or garbage value returned to caller [core.uninitialized.UndefReturn]
+lj_record.c:939:7: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_record.c:1015:18: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_record.c:1015:44: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_record.c:1381:11: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_record.c:2121:7: warning: 1st function call argument is an uninitialized value [core.CallAndMessage]
+lj_record.c:2310:5: warning: 4th function call argument is an uninitialized value [core.CallAndMessage]
+./lj_asm_x86.h:517:11: warning: Branch condition evaluates to a garbage value [core.uninitialized.Branch]
+lj_carith.c:160:7: warning: Access to field 'info' results in a dereference of a null pointer [core.NullDereference]
+lj_lib.c:105:12: warning: Dereference of null pointer [core.NullDereference]
+lib_string.c:294:43: warning: Dereference of null pointer (loaded from variable 's') [core.NullDereference]
+lib_string.c:629:7: warning: Dereference of null pointer [core.NullDereference]
+crypto/asn1/a_object.c:153:24: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+crypto/asn1/f_string.c:130:28: warning: Array access (from variable 's') results in a null pointer dereference [core.NullDereference]
+crypto/asn1/tasn_dec.c:199:16: warning: Access to field 'asn1_ex_d2i' results in a dereference of a null pointer (loaded from variable 'ef') [core.NullDereference]
+crypto/asn1/tasn_enc.c:125:16: warning: Access to field 'asn1_ex_i2d' results in a dereference of a null pointer (loaded from variable 'ef') [core.NullDereference]
+crypto/async/arch/async_posix.h:42:13: warning: Access to field 'env_init' results in a dereference of a null pointer (loaded from variable 'n') [core.NullDereference]
+crypto/async/async_wait.c:157:32: warning: Access to field 'next' results in a dereference of a null pointer (loaded from variable 'prev') [core.NullDereference]
+crypto/bn/bn_exp2.c:178:18: warning: 3rd function call argument is an uninitialized value [core.CallAndMessage]
+crypto/bn/bn_exp2.c:186:18: warning: 3rd function call argument is an uninitialized value [core.CallAndMessage]
+crypto/cms/cms_ess.c:142:30: warning: Access to field 'digestAlgorithm' results in a dereference of a null pointer (loaded from variable 'si') [core.NullDereference]
+crypto/conf/conf_lib.c:295:23: warning: Access to field 'meth' results in a dereference of a null pointer (loaded from variable 'conf') [core.NullDereference]
+crypto/pem/pem_lib.c:560:19: warning: The left expression of the compound assignment is an uninitialized value. The computed value will also be garbage [core.uninitialized.Assign]
+crypto/x509v3/v3_conf.c:315:24: warning: Dereference of null pointer (loaded from variable 'sk') [core.NullDereference]
+engines/afalg/e_afalg.c:761:9: warning: The result of the left shift is undefined because the left operand is negative [core.UndefinedBinaryOperatorResult]
+engines/afalg/e_afalg.c:761:9: warning: The result of the left shift is undefined because the left operand is negative [core.UndefinedBinaryOperatorResult]
+ssl/statem/statem_srvr.c:1890:9: warning: Null pointer passed to 2nd parameter expecting 'nonnull' [core.NonNullParamChecker]
+ssl/t1_lib.c:1804:9: warning: Access to field 'alpn_select_cb' results in a dereference of a null pointer (loaded from field 'ctx') [core.NullDereference]
+apps/s_time.c:270:69: warning: Division by zero [core.DivideZero]
+apps/s_time.c:359:69: warning: Division by zero [core.DivideZero]
+apps/x509.c:910:15: warning: Null pointer passed to 1st parameter expecting 'nonnull' [core.NonNullParamChecker]
+test/evp_test.c:310:33: warning: Array access (from variable 'buf') results in a null pointer dereference [core.NullDereference]
+test/evp_test.c:396:9: warning: Null pointer passed to 1st parameter expecting 'nonnull' [core.NonNullParamChecker]
+test/sslcorrupttest.c:164:39: warning: Array access (from variable 'cipher_list') results in a null pointer dereference [core.NullDereference]
+test/ssltest_old.c:427:10: warning: Null pointer passed to 1st parameter expecting 'nonnull' [core.NonNullParamChecker]
+src/zmalloc.c:105:21: warning: Dereference of null pointer [core.NullDereference]
+src/zmalloc.c:137:21: warning: Dereference of null pointer [core.NullDereference]
+src/zmalloc.c:165:24: warning: Dereference of null pointer [core.NullDereference]
+</t>
+  </si>
   <si>
     <t>no value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lj_bcwrite.c:294:5: warning: Value stored to 'p' is never read [deadcode.DeadStores]
+lj_snap.c:599:8: warning: Value stored to 'tmp' is never read [deadcode.DeadStores]
+lj_crecord.c:248:2: warning: Value stored to 'step' is never read [deadcode.DeadStores]
+./lj_asm_x86.h:1433:11: warning: Although the value stored to 'osrc' is used in the enclosing expression, the value is never actually read from 'osrc' [deadcode.DeadStores]
+lj_cconv.c:212:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:276:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:283:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:289:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:328:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:505:25: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
+crypto/asn1/a_verify.c:68:5: warning: Value stored to 'ret' is never read [deadcode.DeadStores]
+crypto/asn1/a_verify.c:167:5: warning: Value stored to 'ret' is never read [deadcode.DeadStores]
+crypto/asn1/asn_mime.c:571:5: warning: Value stored to 'state' is never read [deadcode.DeadStores]
+crypto/asn1/asn_mime.c:635:13: warning: Although the value stored to 'len' is used in the enclosing expression, the value is never actually read from 'len' [deadcode.DeadStores]
+crypto/asn1/asn_mime.c:968:5: warning: Value stored to 'p' is never read [deadcode.DeadStores]
+crypto/asn1/bio_asn1.c:156:5: warning: Value stored to 'ret' is never read [deadcode.DeadStores]
+crypto/asn1/bio_ndef.c:122:5: warning: Value stored to 'derlen' is never read [deadcode.DeadStores]
+crypto/asn1/tasn_dec.c:330:17: warning: Value stored to 'q' is never read [deadcode.DeadStores]
+crypto/asn1/tasn_dec.c:506:5: warning: Value stored to 'q' is never read [deadcode.DeadStores]
+crypto/bf/bf_cfb64.c:72:5: warning: Value stored to 'v0' is never read [deadcode.DeadStores]
+crypto/bf/bf_cfb64.c:72:10: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/bf/bf_cfb64.c:72:31: warning: Although the value stored to 't' is used in the enclosing expression, the value is never actually read from 't' [deadcode.DeadStores]
+crypto/bf/bf_cfb64.c:72:35: warning: Although the value stored to 'c' is used in the enclosing expression, the value is never actually read from 'c' [deadcode.DeadStores]
+crypto/bf/bf_cfb64.c:72:39: warning: Although the value stored to 'cc' is used in the enclosing expression, the value is never actually read from 'cc' [deadcode.DeadStores]
+crypto/bf/bf_ecb.c:42:5: warning: Value stored to 'l' is never read [deadcode.DeadStores]
+crypto/bf/bf_enc.c:175:5: warning: Value stored to 'tin0' is never read [deadcode.DeadStores]
+crypto/bf/bf_enc.c:175:12: warning: Although the value stored to 'tin1' is used in the enclosing expression, the value is never actually read from 'tin1' [deadcode.DeadStores]
+crypto/bf/bf_enc.c:175:19: warning: Although the value stored to 'tout0' is used in the enclosing expression, the value is never actually read from 'tout0' [deadcode.DeadStores]
+crypto/bf/bf_enc.c:175:27: warning: Although the value stored to 'tout1' is used in the enclosing expression, the value is never actually read from 'tout1' [deadcode.DeadStores]
+crypto/bf/bf_enc.c:175:35: warning: Although the value stored to 'xor0' is used in the enclosing expression, the value is never actually read from 'xor0' [deadcode.DeadStores]
+crypto/bf/bf_enc.c:175:42: warning: Although the value stored to 'xor1' is used in the enclosing expression, the value is never actually read from 'xor1' [deadcode.DeadStores]
+crypto/bf/bf_ofb64.c:59:5: warning: Value stored to 't' is never read [deadcode.DeadStores]
+crypto/bf/bf_ofb64.c:59:9: warning: Although the value stored to 'v0' is used in the enclosing expression, the value is never actually read from 'v0' [deadcode.DeadStores]
+crypto/bf/bf_ofb64.c:59:14: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/bio/b_print.c:331:17: warning: Value stored to 'ch' is never read [deadcode.DeadStores]
+crypto/bio/bss_acpt.c:262:13: warning: Value stored to 's' is never read [deadcode.DeadStores]
+crypto/bio/bss_dgram.c:417:9: warning: Value stored to 'num' is never read [deadcode.DeadStores]
+crypto/bio/bss_dgram.c:498:18: warning: Although the value stored to 'ret' is used in the enclosing expression, the value is never actually read from 'ret' [deadcode.DeadStores]
+crypto/bio/bss_dgram.c:513:18: warning: Although the value stored to 'ret' is used in the enclosing expression, the value is never actually read from 'ret' [deadcode.DeadStores]
+crypto/bn/bn_exp.c:243:5: warning: Value stored to 'wvalue' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:245:5: warning: Value stored to 'wend' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:265:9: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:293:9: warning: Value stored to 'wvalue' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:392:5: warning: Value stored to 'wvalue' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:394:5: warning: Value stored to 'wend' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:431:9: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:459:9: warning: Value stored to 'wvalue' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:1312:5: warning: Value stored to 'wvalue' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:1314:5: warning: Value stored to 'wend' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:1334:9: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+crypto/bn/bn_exp.c:1362:9: warning: Value stored to 'wvalue' is never read [deadcode.DeadStores]
+crypto/bn/bn_mul.c:680:11: warning: Although the value stored to 'zero' is used in the enclosing expression, the value is never actually read from 'zero' [deadcode.DeadStores]
+crypto/bn/bn_mul.c:689:9: warning: Value stored to 'zero' is never read [deadcode.DeadStores]
+crypto/bn/bn_mul.c:699:9: warning: Value stored to 'zero' is never read [deadcode.DeadStores]
+crypto/bn/bn_mul.c:707:9: warning: Value stored to 'zero' is never read [deadcode.DeadStores]
+crypto/bn/bn_mul.c:744:9: warning: Value stored to 'neg' is never read [deadcode.DeadStores]
+crypto/bn/bn_mul.c:747:9: warning: Value stored to 'neg' is never read [deadcode.DeadStores]
+crypto/bn/bn_nist.c:582:9: warning: Value stored to 'carry' is never read [deadcode.DeadStores]
+crypto/bn/bn_nist.c:591:9: warning: Value stored to 'carry' is never read [deadcode.DeadStores]
+crypto/bn/bn_print.c:163:5: warning: Value stored to 'm' is never read [deadcode.DeadStores]
+crypto/cast/c_cfb64.c:72:5: warning: Value stored to 'v0' is never read [deadcode.DeadStores]
+crypto/cast/c_cfb64.c:72:10: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/cast/c_cfb64.c:72:31: warning: Although the value stored to 't' is used in the enclosing expression, the value is never actually read from 't' [deadcode.DeadStores]
+crypto/cast/c_cfb64.c:72:35: warning: Although the value stored to 'c' is used in the enclosing expression, the value is never actually read from 'c' [deadcode.DeadStores]
+crypto/cast/c_cfb64.c:72:39: warning: Although the value stored to 'cc' is used in the enclosing expression, the value is never actually read from 'cc' [deadcode.DeadStores]
+crypto/cast/c_ecb.c:31:5: warning: Value stored to 'l' is never read [deadcode.DeadStores]
+crypto/cast/c_enc.c:149:5: warning: Value stored to 'tin0' is never read [deadcode.DeadStores]
+crypto/cast/c_enc.c:149:12: warning: Although the value stored to 'tin1' is used in the enclosing expression, the value is never actually read from 'tin1' [deadcode.DeadStores]
+crypto/cast/c_enc.c:149:19: warning: Although the value stored to 'tout0' is used in the enclosing expression, the value is never actually read from 'tout0' [deadcode.DeadStores]
+crypto/cast/c_enc.c:149:27: warning: Although the value stored to 'tout1' is used in the enclosing expression, the value is never actually read from 'tout1' [deadcode.DeadStores]
+crypto/cast/c_enc.c:149:35: warning: Although the value stored to 'xor0' is used in the enclosing expression, the value is never actually read from 'xor0' [deadcode.DeadStores]
+crypto/cast/c_enc.c:149:42: warning: Although the value stored to 'xor1' is used in the enclosing expression, the value is never actually read from 'xor1' [deadcode.DeadStores]
+crypto/cast/c_ofb64.c:59:5: warning: Value stored to 't' is never read [deadcode.DeadStores]
+crypto/cast/c_ofb64.c:59:9: warning: Although the value stored to 'v0' is used in the enclosing expression, the value is never actually read from 'v0' [deadcode.DeadStores]
+crypto/cast/c_ofb64.c:59:14: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/cms/cms_pwri.c:61:9: warning: Value stored to 'pbe_nid' is never read [deadcode.DeadStores]
+crypto/des/cbc_cksm.c:44:5: warning: Value stored to 'tout0' is never read [deadcode.DeadStores]
+crypto/des/cbc_cksm.c:44:13: warning: Although the value stored to 'tin0' is used in the enclosing expression, the value is never actually read from 'tin0' [deadcode.DeadStores]
+crypto/des/cbc_cksm.c:44:20: warning: Although the value stored to 'tin1' is used in the enclosing expression, the value is never actually read from 'tin1' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:5: warning: Value stored to 'tin0' is never read [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:12: warning: Although the value stored to 'tin1' is used in the enclosing expression, the value is never actually read from 'tin1' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:19: warning: Although the value stored to 'tout0' is used in the enclosing expression, the value is never actually read from 'tout0' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:27: warning: Although the value stored to 'tout1' is used in the enclosing expression, the value is never actually read from 'tout1' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:35: warning: Although the value stored to 'xor0' is used in the enclosing expression, the value is never actually read from 'xor0' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:42: warning: Although the value stored to 'xor1' is used in the enclosing expression, the value is never actually read from 'xor1' [deadcode.DeadStores]
+crypto/des/cfb64ede.c:77:5: warning: Value stored to 'v0' is never read [deadcode.DeadStores]
+crypto/des/cfb64ede.c:77:10: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/des/cfb64ede.c:77:31: warning: Although the value stored to 'c' is used in the enclosing expression, the value is never actually read from 'c' [deadcode.DeadStores]
+crypto/des/cfb64ede.c:77:35: warning: Although the value stored to 'cc' is used in the enclosing expression, the value is never actually read from 'cc' [deadcode.DeadStores]
+crypto/des/cfb64ede.c:189:5: warning: Value stored to 'v0' is never read [deadcode.DeadStores]
+crypto/des/cfb64ede.c:189:10: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/des/cfb64ede.c:189:15: warning: Although the value stored to 'd0' is used in the enclosing expression, the value is never actually read from 'd0' [deadcode.DeadStores]
+crypto/des/cfb64ede.c:189:20: warning: Although the value stored to 'd1' is used in the enclosing expression, the value is never actually read from 'd1' [deadcode.DeadStores]
+crypto/des/cfb64enc.c:71:5: warning: Value stored to 'v0' is never read [deadcode.DeadStores]
+crypto/des/cfb64enc.c:71:10: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/des/cfb64enc.c:71:31: warning: Although the value stored to 'c' is used in the enclosing expression, the value is never actually read from 'c' [deadcode.DeadStores]
+crypto/des/cfb64enc.c:71:35: warning: Although the value stored to 'cc' is used in the enclosing expression, the value is never actually read from 'cc' [deadcode.DeadStores]
+crypto/des/cfb_enc.c:149:5: warning: Value stored to 'v0' is never read [deadcode.DeadStores]
+crypto/des/cfb_enc.c:149:10: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/des/cfb_enc.c:149:15: warning: Although the value stored to 'd0' is used in the enclosing expression, the value is never actually read from 'd0' [deadcode.DeadStores]
+crypto/des/cfb_enc.c:149:20: warning: Although the value stored to 'd1' is used in the enclosing expression, the value is never actually read from 'd1' [deadcode.DeadStores]
+crypto/des/des_enc.c:83:5: warning: Value stored to 'l' is never read [deadcode.DeadStores]
+crypto/des/des_enc.c:83:9: warning: Although the value stored to 'r' is used in the enclosing expression, the value is never actually read from 'r' [deadcode.DeadStores]
+crypto/des/des_enc.c:83:13: warning: Although the value stored to 't' is used in the enclosing expression, the value is never actually read from 't' [deadcode.DeadStores]
+crypto/des/des_enc.c:83:17: warning: Although the value stored to 'u' is used in the enclosing expression, the value is never actually read from 'u' [deadcode.DeadStores]
+crypto/des/des_enc.c:148:5: warning: Value stored to 'l' is never read [deadcode.DeadStores]
+crypto/des/des_enc.c:148:9: warning: Although the value stored to 'r' is used in the enclosing expression, the value is never actually read from 'r' [deadcode.DeadStores]
+crypto/des/des_enc.c:148:13: warning: Although the value stored to 't' is used in the enclosing expression, the value is never actually read from 't' [deadcode.DeadStores]
+crypto/des/des_enc.c:148:17: warning: Although the value stored to 'u' is used in the enclosing expression, the value is never actually read from 'u' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:5: warning: Value stored to 'tin0' is never read [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:12: warning: Although the value stored to 'tin1' is used in the enclosing expression, the value is never actually read from 'tin1' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:19: warning: Although the value stored to 'tout0' is used in the enclosing expression, the value is never actually read from 'tout0' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:27: warning: Although the value stored to 'tout1' is used in the enclosing expression, the value is never actually read from 'tout1' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:35: warning: Although the value stored to 'xor0' is used in the enclosing expression, the value is never actually read from 'xor0' [deadcode.DeadStores]
+crypto/des/ncbc_enc.c:104:42: warning: Although the value stored to 'xor1' is used in the enclosing expression, the value is never actually read from 'xor1' [deadcode.DeadStores]
+crypto/des/des_enc.c:297:5: warning: Value stored to 'tin0' is never read [deadcode.DeadStores]
+crypto/des/des_enc.c:297:12: warning: Although the value stored to 'tin1' is used in the enclosing expression, the value is never actually read from 'tin1' [deadcode.DeadStores]
+crypto/des/des_enc.c:297:19: warning: Although the value stored to 'tout0' is used in the enclosing expression, the value is never actually read from 'tout0' [deadcode.DeadStores]
+crypto/des/des_enc.c:297:27: warning: Although the value stored to 'tout1' is used in the enclosing expression, the value is never actually read from 'tout1' [deadcode.DeadStores]
+crypto/des/des_enc.c:297:35: warning: Although the value stored to 'xor0' is used in the enclosing expression, the value is never actually read from 'xor0' [deadcode.DeadStores]
+crypto/des/des_enc.c:297:42: warning: Although the value stored to 'xor1' is used in the enclosing expression, the value is never actually read from 'xor1' [deadcode.DeadStores]
+crypto/des/ecb_enc.c:50:5: warning: Value stored to 'l' is never read [deadcode.DeadStores]
+crypto/des/ofb64ede.c:60:5: warning: Value stored to 'v0' is never read [deadcode.DeadStores]
+crypto/des/ofb64ede.c:60:10: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/des/ofb64enc.c:58:5: warning: Value stored to 't' is never read [deadcode.DeadStores]
+crypto/des/ofb64enc.c:58:9: warning: Although the value stored to 'v0' is used in the enclosing expression, the value is never actually read from 'v0' [deadcode.DeadStores]
+crypto/des/ofb64enc.c:58:14: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/des/ofb_enc.c:81:5: warning: Value stored to 'v0' is never read [deadcode.DeadStores]
+crypto/des/ofb_enc.c:81:10: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/des/ofb_enc.c:81:15: warning: Although the value stored to 'd0' is used in the enclosing expression, the value is never actually read from 'd0' [deadcode.DeadStores]
+crypto/des/ofb_enc.c:81:20: warning: Although the value stored to 'd1' is used in the enclosing expression, the value is never actually read from 'd1' [deadcode.DeadStores]
+crypto/des/ofb_enc.c:81:41: warning: Although the value stored to 'vv0' is used in the enclosing expression, the value is never actually read from 'vv0' [deadcode.DeadStores]
+crypto/des/ofb_enc.c:81:47: warning: Although the value stored to 'vv1' is used in the enclosing expression, the value is never actually read from 'vv1' [deadcode.DeadStores]
+crypto/des/pcbc_enc.c:65:5: warning: Value stored to 'sin0' is never read [deadcode.DeadStores]
+crypto/des/pcbc_enc.c:65:12: warning: Although the value stored to 'sin1' is used in the enclosing expression, the value is never actually read from 'sin1' [deadcode.DeadStores]
+crypto/des/pcbc_enc.c:65:19: warning: Although the value stored to 'xor0' is used in the enclosing expression, the value is never actually read from 'xor0' [deadcode.DeadStores]
+crypto/des/pcbc_enc.c:65:26: warning: Although the value stored to 'xor1' is used in the enclosing expression, the value is never actually read from 'xor1' [deadcode.DeadStores]
+crypto/des/pcbc_enc.c:65:33: warning: Although the value stored to 'tout0' is used in the enclosing expression, the value is never actually read from 'tout0' [deadcode.DeadStores]
+crypto/des/pcbc_enc.c:65:41: warning: Although the value stored to 'tout1' is used in the enclosing expression, the value is never actually read from 'tout1' [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:100:5: warning: Value stored to 'tin0' is never read [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:100:12: warning: Although the value stored to 'tin1' is used in the enclosing expression, the value is never actually read from 'tin1' [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:100:19: warning: Although the value stored to 'tout0' is used in the enclosing expression, the value is never actually read from 'tout0' [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:100:27: warning: Although the value stored to 'tout1' is used in the enclosing expression, the value is never actually read from 'tout1' [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:100:35: warning: Although the value stored to 'xor0' is used in the enclosing expression, the value is never actually read from 'xor0' [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:100:42: warning: Although the value stored to 'xor1' is used in the enclosing expression, the value is never actually read from 'xor1' [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:101:5: warning: Value stored to 'inW0' is never read [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:101:12: warning: Although the value stored to 'inW1' is used in the enclosing expression, the value is never actually read from 'inW1' [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:101:19: warning: Although the value stored to 'outW0' is used in the enclosing expression, the value is never actually read from 'outW0' [deadcode.DeadStores]
+crypto/des/xcbc_enc.c:101:27: warning: Although the value stored to 'outW1' is used in the enclosing expression, the value is never actually read from 'outW1' [deadcode.DeadStores]
+crypto/ec/ec_mult.c:294:17: warning: Value stored to 'numblocks' is never read [deadcode.DeadStores]
+crypto/engine/eng_dyn.c:218:13: warning: Value stored to 'new_idx' is never read [deadcode.DeadStores]
+crypto/evp/e_aes_cbc_hmac_sha1.c:711:17: warning: Value stored to 'maxpad' is never read [deadcode.DeadStores]
+crypto/evp/e_aes_cbc_hmac_sha256.c:716:17: warning: Value stored to 'maxpad' is never read [deadcode.DeadStores]
+crypto/objects/obj_dat.c:516:13: warning: Value stored to 'l' is never read [deadcode.DeadStores]
+crypto/rc2/rc2_cbc.c:84:5: warning: Value stored to 'tin0' is never read [deadcode.DeadStores]
+crypto/rc2/rc2_cbc.c:84:12: warning: Although the value stored to 'tin1' is used in the enclosing expression, the value is never actually read from 'tin1' [deadcode.DeadStores]
+crypto/rc2/rc2_cbc.c:84:19: warning: Although the value stored to 'tout0' is used in the enclosing expression, the value is never actually read from 'tout0' [deadcode.DeadStores]
+crypto/rc2/rc2_cbc.c:84:27: warning: Although the value stored to 'tout1' is used in the enclosing expression, the value is never actually read from 'tout1' [deadcode.DeadStores]
+crypto/rc2/rc2_cbc.c:84:35: warning: Although the value stored to 'xor0' is used in the enclosing expression, the value is never actually read from 'xor0' [deadcode.DeadStores]
+crypto/rc2/rc2_cbc.c:84:42: warning: Although the value stored to 'xor1' is used in the enclosing expression, the value is never actually read from 'xor1' [deadcode.DeadStores]
+crypto/rc2/rc2_ecb.c:40:5: warning: Value stored to 'l' is never read [deadcode.DeadStores]
+crypto/rc2/rc2cfb64.c:72:5: warning: Value stored to 'v0' is never read [deadcode.DeadStores]
+crypto/rc2/rc2cfb64.c:72:10: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/rc2/rc2cfb64.c:72:31: warning: Although the value stored to 't' is used in the enclosing expression, the value is never actually read from 't' [deadcode.DeadStores]
+crypto/rc2/rc2cfb64.c:72:35: warning: Although the value stored to 'c' is used in the enclosing expression, the value is never actually read from 'c' [deadcode.DeadStores]
+crypto/rc2/rc2cfb64.c:72:39: warning: Although the value stored to 'cc' is used in the enclosing expression, the value is never actually read from 'cc' [deadcode.DeadStores]
+crypto/rc2/rc2ofb64.c:59:5: warning: Value stored to 't' is never read [deadcode.DeadStores]
+crypto/rc2/rc2ofb64.c:59:9: warning: Although the value stored to 'v0' is used in the enclosing expression, the value is never actually read from 'v0' [deadcode.DeadStores]
+crypto/rc2/rc2ofb64.c:59:14: warning: Although the value stored to 'v1' is used in the enclosing expression, the value is never actually read from 'v1' [deadcode.DeadStores]
+crypto/ts/ts_rsp_verify.c:136:13: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
+crypto/txt_db/txt_db.c:83:9: warning: Value stored to 'i' is never read [deadcode.DeadStores]
+crypto/x509/x509_vfy.c:3081:61: warning: Although the value stored to 'x' is used in the enclosing expression, the value is never actually read from 'x' [deadcode.DeadStores]
+crypto/x509/x509_vfy.c:3164:25: warning: Although the value stored to 'x' is used in the enclosing expression, the value is never actually read from 'x' [deadcode.DeadStores]
+ssl/statem/statem_clnt.c:2574:5: warning: Value stored to 'pmslen' is never read [deadcode.DeadStores]
+ssl/statem/statem_lib.c:1058:24: warning: Although the value stored to 'single' is used in the enclosing expression, the value is never actually read from 'single' [deadcode.DeadStores]
+ssl/statem/statem_srvr.c:1448:9: warning: Value stored to 'wst' is never read [deadcode.DeadStores]
+apps/apps.c:1391:9: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1434:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1435:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1570:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1571:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1572:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1619:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1620:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1621:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1622:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/apps.c:1623:5: warning: Value stored to 'j' is never read [deadcode.DeadStores]
+apps/cms.c:586:5: warning: Value stored to 'argc' is never read [deadcode.DeadStores]
+apps/dhparam.c:138:5: warning: Value stored to 'argc' is never read [deadcode.DeadStores]
+apps/dsaparam.c:275:13: warning: Value stored to 'i' is never read [deadcode.DeadStores]
+apps/dsaparam.c:277:13: warning: Value stored to 'i' is never read [deadcode.DeadStores]
+apps/ecparam.c:439:13: warning: Value stored to 'i' is never read [deadcode.DeadStores]
+apps/ecparam.c:441:13: warning: Value stored to 'i' is never read [deadcode.DeadStores]
+apps/engine.c:328:5: warning: Value stored to 'argc' is never read [deadcode.DeadStores]
+apps/genrsa.c:111:5: warning: Value stored to 'argc' is never read [deadcode.DeadStores]
+apps/openssl.c:191:39: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
+apps/passwd.c:142:5: warning: Value stored to 'argc' is never read [deadcode.DeadStores]
+apps/passwd.c:148:9: warning: Value stored to 'pw_source_defined' is never read [deadcode.DeadStores]
+apps/rehash.c:496:5: warning: Value stored to 'argc' is never read [deadcode.DeadStores]
+apps/s_cb.c:1037:10: warning: Although the value stored to 'mdpth' is used in the enclosing expression, the value is never actually read from 'mdpth' [deadcode.DeadStores]
+apps/s_client.c:1838:5: warning: Value stored to 'tty_on' is never read [deadcode.DeadStores]
+apps/s_server.c:1437:5: warning: Value stored to 'argc' is never read [deadcode.DeadStores]
+apps/s_server.c:1438:5: warning: Value stored to 'argv' is never read [deadcode.DeadStores]
+apps/s_server.c:2230:21: warning: Value stored to 'i' is never read [deadcode.DeadStores]
+apps/s_server.c:2243:21: warning: Value stored to 'i' is never read [deadcode.DeadStores]
+apps/s_server.c:2261:17: warning: Although the value stored to 'k' is used in the enclosing expression, the value is never actually read from 'k' [deadcode.DeadStores]
+apps/s_time.c:264:5: warning: Value stored to 'i' is never read [deadcode.DeadStores]
+test/asynciotest.c:306:18: warning: Value stored to 'ret' is never read [deadcode.DeadStores]
+test/asynciotest.c:333:18: warning: Value stored to 'ret' is never read [deadcode.DeadStores]
+test/bftest.c:401:35: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
+test/evp_test.c:833:25: warning: Value stored to 'cdat' during its initialization is never read [deadcode.DeadStores]
+test/packettest.c:508:5: warning: Value stored to 'i' is never read [deadcode.DeadStores]
+test/ssltest_old.c:2183:9: warning: Value stored to 'ret' is never read [deadcode.DeadStores]
+test/ssltest_old.c:2566:9: warning: Value stored to 'ret' is never read [deadcode.DeadStores]
+</t>
+  </si>
+  <si>
+    <t>include/openssl/engine.h:255:16: warning: Excessive padding in 'struct ENGINE_CMD_DEFN_st' (8 padding bytes, where 0 is optimal). Optimal fields order: cmd_name, cmd_desc, cmd_num, cmd_flags, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+crypto/x509/x509_lcl.h:16:8: warning: Excessive padding in 'struct X509_VERIFY_PARAM_st' (8 padding bytes, where 0 is optimal). Optimal fields order: name, check_time, flags, policies, hosts, peername, email, emaillen, ip, iplen, inh_flags, purpose, trust, depth, auth_level, hostflags, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/record/../ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/record/../ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/record/../record/record.h:32:16: warning: Excessive padding in 'struct ssl3_record_st' (8 padding bytes, where 0 is optimal). Optimal fields order: data, input, comp, epoch, rec_version, type, length, orig_len, off, read, seq_num, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/record/../ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/record/../ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/record/../ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:416:8: warning: Excessive padding in 'struct ssl_cipher_st' (8 padding bytes, where 0 is optimal). Optimal fields order: name, valid, id, algorithm_mkey, algorithm_auth, algorithm_enc, algorithm_mac, min_tls, max_tls, min_dtls, max_dtls, algo_strength, algorithm2, strength_bits, alg_bits, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback, ctx, verified_chain, verify_result, ex_data, client_CA, max_cert_list, tlsext_debug_cb, tlsext_debug_arg, tlsext_hostname, ct_validation_callback, ct_validation_callback_arg, scts, tlsext_scts, tlsext_ocsp_ids, tlsext_ocsp_exts, tlsext_ocsp_resp, tlsext_ecpointformatlist_length, tlsext_ecpointformatlist, tlsext_ellipticcurvelist_length, tlsext_ellipticcurvelist, tlsext_session_ticket, tls_session_ticket_ext_cb, tls_session_ticket_ext_cb_arg, tls_session_secret_cb, tls_session_secret_cb_arg, session_ctx, next_proto_negotiated, srtp_profiles, srtp_profile, alpn_client_proto_list, not_resumable_session_cb, default_passwd_callback, default_passwd_callback_userdata, job, waitctx, lock, dane, rlayer, version, rwstate, server, new_session, quiet_shutdown, shutdown, init_num, init_off, hit, mac_flags, sid_ctx_length, verify_mode, error, error_code, references, options, mode, min_proto_version, max_proto_version, first_packet, client_version, split_send_fragment, max_send_fragment, max_pipelines, servername_done, tlsext_status_type, scts_parsed, tlsext_status_expected, tlsext_ocsp_resplen, tlsext_ticket_expected, tlsext_heartbeat, tlsext_hb_pending, tlsext_hb_seq, alpn_client_proto_list_len, tlsext_use_etm, renegotiate, statem, tlsext_scts_len, next_proto_negotiated_len, sid_ctx, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:416:8: warning: Excessive padding in 'struct ssl_cipher_st' (8 padding bytes, where 0 is optimal). Optimal fields order: name, valid, id, algorithm_mkey, algorithm_auth, algorithm_enc, algorithm_mac, min_tls, max_tls, min_dtls, max_dtls, algo_strength, algorithm2, strength_bits, alg_bits, consider reordering the fields or adding explicit padding members [optin.performance.Padding]
+ssl/ssl_locl.h:875:8: warning: Excessive padding in 'struct ssl_st' (57 padding bytes, where 1 is optimal). Optimal fields order: method, rbio, wbio, bbio, handshake_func, init_buf, init_msg, s3, d1, msg_callback, msg_callback_arg, param, cipher_list, cipher_list_by_id, enc_read_ctx, read_hash, compress, expand, enc_write_ctx, write_hash, cert, session, generate_session_id, verify_callback, info_callback,</t>
+  </si>
+  <si>
+    <t>host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:104:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:199:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:698:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:733:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:742:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:745:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:747:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:753:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:755:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:756:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:760:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1295:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1352:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4704:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4905:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6102:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6762:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7568:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7576:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7601:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7606:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7611:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7616:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7632:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:140:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:141:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:145:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:163:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:170:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:189:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:198:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:206:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:222:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:46:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:63:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:94:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:142:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:201:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:225:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:254:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_buf.c:214:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_buf.c:215:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:104:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:199:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:323:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:332:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:340:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:341:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:343:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:345:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_state.c:193:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:148:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1394:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1485:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:61:18: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:64:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:79:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:116:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:98:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:106:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_opt_dce.c:72:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./lj_buf.h:75:18: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:210:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:751:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:862:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:863:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:1922:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:1924:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2540:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2541:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2545:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ffrecord.c:111:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ffrecord.c:120:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ffrecord.c:136:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:312:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:2372:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apps/rehash.c:353:21: warning: Potential leak of memory pointed to by 'copy' [unix.Malloc]
+</t>
   </si>
 </sst>
 </file>
@@ -351,7 +759,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B20:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,9 +768,39 @@
     <col min="3" max="12" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="20" spans="2:12">
+      <c r="B20" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel test ver 8
</commit_message>
<xml_diff>
--- a/c_wrk/test.xlsx
+++ b/c_wrk/test.xlsx
@@ -14,7 +14,1052 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="43">
+  <si>
+    <t>2012-03-18T06:39:52Z_1.0.0</t>
+  </si>
+  <si>
+    <t>no value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">src/http_parser.c:1950:3: warning: Value stored to 'uf' is never read [deadcode.DeadStores]
+</t>
+  </si>
+  <si>
+    <t>2013-02-16T08:20:50Z_1.1.0</t>
+  </si>
+  <si>
+    <t>2013-03-03T10:15:57Z_1.1.1</t>
+  </si>
+  <si>
+    <t>2013-04-07T05:37:24Z_1.2.0</t>
+  </si>
+  <si>
+    <t>2013-04-21T08:24:10Z_2.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">src/http_parser.c:2070:3: warning: Value stored to 'uf' is never read [deadcode.DeadStores]
+</t>
+  </si>
+  <si>
+    <t>2013-06-22T07:37:46Z_2.2.0</t>
+  </si>
+  <si>
+    <t>2013-06-26T07:28:25Z_2.2.1</t>
+  </si>
+  <si>
+    <t>2013-06-30T14:08:43Z_2.2.2</t>
+  </si>
+  <si>
+    <t>2013-09-22T04:05:06Z_3.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host/minilua.c:4348:10: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
+host/minilua.c:4590:9: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_strscan.c:309:7: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_opt_mem.c:46:9: warning: Dereference of null pointer [core.NullDereference]
+lj_opt_narrow.c:374:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
+lj_opt_narrow.c:375:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
+./lj_obj.h:842:5: warning: Undefined or garbage value returned to caller [core.uninitialized.UndefReturn]
+lj_record.c:808:7: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_record.c:878:11: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_record.c:878:30: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_record.c:1166:11: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_record.c:1783:7: warning: 1st function call argument is an uninitialized value [core.CallAndMessage]
+./lj_asm_x86.h:395:11: warning: Branch condition evaluates to a garbage value [core.uninitialized.Branch]
+./lj_asm_x86.h:455:5: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_carith.c:158:7: warning: Access to field 'info' results in a dereference of a null pointer [core.NullDereference]
+lj_lib.c:80:12: warning: Dereference of null pointer [core.NullDereference]
+lib_string.c:324:43: warning: Dereference of null pointer (loaded from variable 's') [core.NullDereference]
+lib_string.c:687:7: warning: Dereference of null pointer [core.NullDereference]
+luajit.c:284:34: warning: Null pointer passed to 1st parameter expecting 'nonnull' [core.NonNullParamChecker]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lj_snap.c:566:8: warning: Value stored to 'tmp' is never read [deadcode.DeadStores]
+lj_crecord.c:247:2: warning: Value stored to 'step' is never read [deadcode.DeadStores]
+./lj_asm_x86.h:1293:11: warning: Although the value stored to 'osrc' is used in the enclosing expression, the value is never actually read from 'osrc' [deadcode.DeadStores]
+lj_cconv.c:212:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:276:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:283:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:289:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:328:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:503:25: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
+src/http_parser.c:2070:3: warning: Value stored to 'uf' is never read [deadcode.DeadStores]
+</t>
+  </si>
+  <si>
+    <t>host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:697:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:732:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:741:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:744:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:746:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:752:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:754:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:755:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:758:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1294:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1351:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4703:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4904:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6101:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6761:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7567:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7575:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7600:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7605:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7610:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7615:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7631:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1388:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1511:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:181:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:650:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:753:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:754:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2151:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2152:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2153:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:285:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:291:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:315:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:361:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:413:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:479:40: warning: Call to function 'memcpy' is insecure as it does not provide security chec</t>
+  </si>
+  <si>
+    <t>2013-10-05T05:25:16Z_3.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:697:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:732:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:741:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:744:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:746:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:752:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:754:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:755:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:758:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1294:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1351:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4703:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4904:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6101:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6761:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7567:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7575:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7600:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7605:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7610:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7615:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7631:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1388:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1511:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:181:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:650:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:753:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:754:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2151:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2152:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2153:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:285:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:291:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:315:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:361:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:413:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:479:40: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:481:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:529:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:582:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:678:36: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:680:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 </t>
+  </si>
+  <si>
+    <t>2013-11-09T03:30:53Z_3.0.2</t>
+  </si>
+  <si>
+    <t>2013-11-10T07:23:14Z_3.0.3</t>
+  </si>
+  <si>
+    <t>2013-11-16T03:06:29Z_3.0.4</t>
+  </si>
+  <si>
+    <t>host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:697:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:732:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:741:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:744:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:746:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:752:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:754:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:755:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:758:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1294:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1351:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4703:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4904:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6101:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6761:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7567:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7575:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7600:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7605:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7610:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7615:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7631:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1388:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1511:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:181:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:650:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:753:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:754:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2151:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2152:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2153:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:285:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:291:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:315:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:361:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:413:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:479:40: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:481:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:529:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:582:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:678:36: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:680:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:714:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:740:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:554:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:572:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:670:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:672:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with a</t>
+  </si>
+  <si>
+    <t>2014-02-10T10:35:13Z_3.1.0</t>
+  </si>
+  <si>
+    <t>host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:697:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:732:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:741:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:744:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:746:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:752:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:754:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:755:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:758:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1294:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1351:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4703:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4904:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6101:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6761:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7567:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7575:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7600:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7605:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7610:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7615:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7631:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:328:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:337:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:342:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:345:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:346:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:348:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:350:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1388:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1511:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:181:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:650:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:753:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:754:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2151:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2152:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2153:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides bo</t>
+  </si>
+  <si>
+    <t>2014-08-05T12:50:32Z_3.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host/minilua.c:4349:10: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
+host/minilua.c:4591:9: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_strscan.c:309:7: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_opt_mem.c:46:9: warning: Dereference of null pointer [core.NullDereference]
+lj_opt_narrow.c:374:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
+lj_opt_narrow.c:375:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
+./lj_obj.h:842:5: warning: Undefined or garbage value returned to caller [core.uninitialized.UndefReturn]
+lj_record.c:810:7: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_record.c:880:11: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_record.c:880:30: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_record.c:1168:11: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_record.c:1784:7: warning: 1st function call argument is an uninitialized value [core.CallAndMessage]
+./lj_asm_x86.h:395:11: warning: Branch condition evaluates to a garbage value [core.uninitialized.Branch]
+./lj_asm_x86.h:455:5: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_carith.c:158:7: warning: Access to field 'info' results in a dereference of a null pointer [core.NullDereference]
+lj_lib.c:80:12: warning: Dereference of null pointer [core.NullDereference]
+lib_string.c:324:43: warning: Dereference of null pointer (loaded from variable 's') [core.NullDereference]
+lib_string.c:687:7: warning: Dereference of null pointer [core.NullDereference]
+luajit.c:284:34: warning: Null pointer passed to 1st parameter expecting 'nonnull' [core.NonNullParamChecker]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lj_snap.c:566:8: warning: Value stored to 'tmp' is never read [deadcode.DeadStores]
+lj_crecord.c:247:2: warning: Value stored to 'step' is never read [deadcode.DeadStores]
+./lj_asm_x86.h:1294:11: warning: Although the value stored to 'osrc' is used in the enclosing expression, the value is never actually read from 'osrc' [deadcode.DeadStores]
+lj_cconv.c:212:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:276:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:283:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:289:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:328:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:503:25: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
+src/http_parser.c:2070:3: warning: Value stored to 'uf' is never read [deadcode.DeadStores]
+</t>
+  </si>
+  <si>
+    <t>host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:335:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:344:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:349:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:352:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:353:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:355:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:357:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:698:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:733:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:742:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:745:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:747:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:753:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:755:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:756:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:760:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1295:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1352:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4704:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4905:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6102:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6762:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7568:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7576:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7601:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7606:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7611:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7616:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7632:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:335:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:344:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:349:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:352:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:353:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:355:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:357:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1388:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1511:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:181:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:650:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:755:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:756:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2152:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2153:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2154:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:285:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:291:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:315:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provide</t>
+  </si>
+  <si>
+    <t>2015-01-31T05:54:36Z_3.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lj_snap.c:566:8: warning: Value stored to 'tmp' is never read [deadcode.DeadStores]
+lj_crecord.c:247:2: warning: Value stored to 'step' is never read [deadcode.DeadStores]
+./lj_asm_x86.h:1294:11: warning: Although the value stored to 'osrc' is used in the enclosing expression, the value is never actually read from 'osrc' [deadcode.DeadStores]
+lj_cconv.c:212:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:276:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:283:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:289:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:328:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:503:25: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
+</t>
+  </si>
+  <si>
+    <t>host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:335:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:344:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:349:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:352:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:353:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:355:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:357:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:698:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:733:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:742:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:745:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:747:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:753:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:755:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:756:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:760:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1295:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1352:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4704:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4905:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6102:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6762:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7568:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7576:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7601:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7606:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7611:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7616:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7632:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:335:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:344:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:349:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:352:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:353:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:355:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:357:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1388:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1511:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:181:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:650:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:755:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:756:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2152:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2153:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2154:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:285:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:291:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:315:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:361:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:413:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:479:40: warning: Call to function 'memcpy' is insecure as it does not provide security chec</t>
+  </si>
+  <si>
+    <t>2015-03-18T12:18:33Z_4.0.0</t>
+  </si>
+  <si>
+    <t>2015-03-24T10:03:52Z_4.0.1</t>
+  </si>
+  <si>
+    <t>host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:698:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:733:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:742:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:745:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:747:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:753:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:755:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:756:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:760:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1295:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1352:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4704:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4905:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6102:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6762:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7568:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7576:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7601:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7606:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7611:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7616:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7632:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:335:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:344:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:349:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:352:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:353:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:355:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:357:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1388:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1511:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:181:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:650:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:755:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:756:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2152:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2153:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2154:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:285:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:291:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:315:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:361:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:413:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:479:40: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:481:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:529:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:582:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:678:36: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:680:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:714:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:740:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:555:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:573:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:671:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:673:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with a</t>
+  </si>
+  <si>
+    <t>2016-03-26T00:18:07Z_4.0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host/minilua.c:4349:10: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
+host/minilua.c:4591:9: warning: The left operand of '==' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_strscan.c:295:5: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_strscan.c:310:7: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_opt_mem.c:46:9: warning: Dereference of null pointer [core.NullDereference]
+lj_opt_narrow.c:382:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
+lj_opt_narrow.c:383:8: warning: 2nd function call argument is an uninitialized value [core.CallAndMessage]
+./lj_obj.h:842:5: warning: Undefined or garbage value returned to caller [core.uninitialized.UndefReturn]
+lj_record.c:813:7: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_record.c:883:11: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_record.c:883:30: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_record.c:1171:11: warning: The left operand of '&amp;' is a garbage value [core.UndefinedBinaryOperatorResult]
+lj_record.c:1787:7: warning: 1st function call argument is an uninitialized value [core.CallAndMessage]
+./lj_asm_x86.h:403:11: warning: Branch condition evaluates to a garbage value [core.uninitialized.Branch]
+./lj_asm_x86.h:463:5: warning: Assigned value is garbage or undefined [core.uninitialized.Assign]
+lj_carith.c:158:7: warning: Access to field 'info' results in a dereference of a null pointer [core.NullDereference]
+lj_lib.c:80:12: warning: Dereference of null pointer [core.NullDereference]
+lib_string.c:324:43: warning: Dereference of null pointer (loaded from variable 's') [core.NullDereference]
+lib_string.c:687:7: warning: Dereference of null pointer [core.NullDereference]
+luajit.c:284:34: warning: Null pointer passed to 1st parameter expecting 'nonnull' [core.NonNullParamChecker]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lj_snap.c:567:8: warning: Value stored to 'tmp' is never read [deadcode.DeadStores]
+lj_crecord.c:247:2: warning: Value stored to 'step' is never read [deadcode.DeadStores]
+./lj_asm_x86.h:1302:11: warning: Although the value stored to 'osrc' is used in the enclosing expression, the value is never actually read from 'osrc' [deadcode.DeadStores]
+lj_cconv.c:212:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:276:5: warning: Value stored to 'sinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:283:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:289:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:328:5: warning: Value stored to 'dinfo' is never read [deadcode.DeadStores]
+lj_cconv.c:503:25: warning: Although the value stored to 'i' is used in the enclosing expression, the value is never actually read from 'i' [deadcode.DeadStores]
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:698:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:733:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:742:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:745:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:747:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:753:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:755:1: warning: Call to function 'strncat' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncat_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:756:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:759:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:760:1: warning: Call to function 'strcat' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcat'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:1295:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:1352:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4704:1: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:4905:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6102:1: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:6762:4: warning: Call to function 'fscanf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'fscanf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7568:1: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7576:1: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/minilua.c:7601:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7606:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7611:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7616:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/minilua.c:7632:1: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:134:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:145:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+./../dynasm/dasm_x86.h:146:20: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:108:3: warning: Call to function 'sprintf' is insecure as it does not provide bounding of the memory buffer or security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm.c:123:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm.c:178:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:138:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:139:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:143:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:161:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:168:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:186:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:187:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:196:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:204:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_peobj.c:213:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:44:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:61:12: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_lib.c:92:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:140:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:167:3: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+host/buildvm_lib.c:196:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+host/buildvm_fold.c:22:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:76:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:152:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_str.c:180:20: warning: Call to function 'sprintf' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'sprintf_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_tab.c:179:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_meta.c:298:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:337:5: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:346:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:351:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:354:7: warning: Call to function 'strncpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'strncpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_debug.c:355:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:357:7: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_debug.c:359:5: warning: Call to function 'strcpy' is insecure as it does not provide bounding of the memory buffer. Replace unbounded copy functions with analogous functions that support length arguments such as 'strlcpy'. CWE-119 [security.insecureAPI.strcpy]
+lj_state.c:188:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_dispatch.c:133:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1390:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_parse.c:1513:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:69:4: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:72:2: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:86:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_bcread.c:125:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:96:5: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ir.c:104:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_opt_dce.c:72:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_snap.c:182:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:651:3: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:758:7: warning: Call to function 'memmove' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memmove_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:759:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2155:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2156:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_record.c:2157:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_asm.c:304:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:130:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:136:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:138:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:139:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:277:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:280:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_trace.c:385:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ctype.c:595:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:169:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:170:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:178:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:285:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:291:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:315:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:361:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:413:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:479:40: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:481:7: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:529:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:582:7: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:678:36: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:680:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:715:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_cconv.c:741:5: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memset_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:555:5: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:573:3: warning: Call to function 'memcpy' is insecure as it does not provide security checks introduced in the C11 standard. Replace with analogous functions that support length arguments or provides boundary checks such as 'memcpy_s' in case of C11 [security.insecureAPI.DeprecatedOrUnsafeBufferHandling]
+lj_ccall.c:671:3: warning: Call to function 'memset' is insecure as it does not provide security checks introduced in the C11 standard. Replace with </t>
+  </si>
   <si>
     <t>2018-01-21T06:00:58Z_4.1.0</t>
   </si>
@@ -69,9 +1114,6 @@
 src/zmalloc.c:137:21: warning: Dereference of null pointer [core.NullDereference]
 src/zmalloc.c:165:24: warning: Dereference of null pointer [core.NullDereference]
 </t>
-  </si>
-  <si>
-    <t>no value</t>
   </si>
   <si>
     <t xml:space="preserve">lj_bcwrite.c:294:5: warning: Value stored to 'p' is never read [deadcode.DeadStores]
@@ -759,7 +1801,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B20:L20"/>
+  <dimension ref="B1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -768,39 +1810,704 @@
     <col min="3" max="12" width="100.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:12">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="20" spans="2:12">
       <c r="B20" s="1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel test ver 10
</commit_message>
<xml_diff>
--- a/c_wrk/test.xlsx
+++ b/c_wrk/test.xlsx
@@ -14,7 +14,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="54">
+  <si>
+    <t>date &amp; version</t>
+  </si>
+  <si>
+    <t>core</t>
+  </si>
+  <si>
+    <t>cplusplus</t>
+  </si>
+  <si>
+    <t>deadcode</t>
+  </si>
+  <si>
+    <t>nullability</t>
+  </si>
+  <si>
+    <t>optin</t>
+  </si>
+  <si>
+    <t>security</t>
+  </si>
+  <si>
+    <t>unix</t>
+  </si>
+  <si>
+    <t>osx</t>
+  </si>
+  <si>
+    <t>fuchsia</t>
+  </si>
+  <si>
+    <t>webkit</t>
+  </si>
   <si>
     <t>2012-03-18T06:39:52Z_1.0.0</t>
   </si>
@@ -1801,13 +1834,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L20"/>
+  <dimension ref="B1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="12" width="100.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12">
@@ -1818,696 +1851,731 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="2:12">
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:12">
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:12">
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:12">
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:12">
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:12">
       <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:12">
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:12">
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:12">
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>